<commit_message>
added a way for user to select the excel worksheet
</commit_message>
<xml_diff>
--- a/Files/SAMPLE.xlsx
+++ b/Files/SAMPLE.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6962855C-9260-45B4-B1A3-9A53F8CA4F65}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244B2499-5791-422B-9DAC-CDDCFA32FE2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CA4EE278-4183-4866-B694-D2430B14ABD9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="carsSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="laptopSheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Corolla</t>
   </si>
@@ -87,6 +88,45 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Dell</t>
+  </si>
+  <si>
+    <t>Inspiron 15</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Pavilion x360</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>MacBook Pro</t>
+  </si>
+  <si>
+    <t>Space Gray</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>ThinkPad X1 Carbon</t>
+  </si>
+  <si>
+    <t>Acer</t>
+  </si>
+  <si>
+    <t>Swift 3</t>
+  </si>
+  <si>
+    <t>Gray</t>
   </si>
 </sst>
 </file>
@@ -450,7 +490,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F12" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,4 +583,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453985A5-0049-477B-B6B6-3BE41B1ED319}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a few validations
- added a way for user to input the SQL server name and database name dynamically instead of the static initialization in the code before
 - displays an error message if the SQL server name or database name is incorrect or doesn't exist
 - displays an error message if there is a mismatch of data type between the excel data and SQL column (i.e. excel data is a text but SQL column is an int)
</commit_message>
<xml_diff>
--- a/Files/SAMPLE.xlsx
+++ b/Files/SAMPLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244B2499-5791-422B-9DAC-CDDCFA32FE2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5462BD1-8A03-4F58-BD1C-9518D8E8DAF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CA4EE278-4183-4866-B694-D2430B14ABD9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CA4EE278-4183-4866-B694-D2430B14ABD9}"/>
   </bookViews>
   <sheets>
     <sheet name="carsSheet" sheetId="1" r:id="rId1"/>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C9087C-E89B-4CB0-9A84-2E7020B30019}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F11:F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453985A5-0049-477B-B6B6-3BE41B1ED319}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>